<commit_message>
Add new files and updates
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -647,6 +647,23 @@
         <v>1242.699081698724</v>
       </c>
     </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2.250477639167457</v>
+      </c>
+      <c r="C16">
+        <v>44.89971791433486</v>
+      </c>
+      <c r="D16">
+        <v>17.74952915753526</v>
+      </c>
+      <c r="E16">
+        <v>1244.949559337892</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>